<commit_message>
Commit para actualizar data
</commit_message>
<xml_diff>
--- a/E-Commerce_test.xlsx
+++ b/E-Commerce_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Henry\Datathon\E-Comerce\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aagui\Github\Datathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2813B76-6757-40B6-ACC7-8F97E1B404B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82EAA8F-A2AC-4AE3-946B-BB7C8FFA512F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5010" yWindow="690" windowWidth="14175" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -129,8 +129,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,46 +417,51 @@
   <dimension ref="A1:K2001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="A2001" sqref="A2001"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
     <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>